<commit_message>
ajout algo + eval
Ajout de la lecture de la fonction d'evaluation et de l'algorithme depuis le fichier excel
</commit_message>
<xml_diff>
--- a/tsume-configuration.xlsx
+++ b/tsume-configuration.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mes docs\Documents\Mes documents\home\quicklisp\local-projects\TsumeLi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072740B9-4C97-4B25-877C-F34300423174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8866D-7CDA-44AC-A20E-0FB9414A2806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Ce tableur permet la saisie de la configuration du tsume qui sera résolu par le programme TsumeLi</t>
   </si>
@@ -64,19 +64,45 @@
   </si>
   <si>
     <t>-P</t>
+  </si>
+  <si>
+    <t>Evaluation function</t>
+  </si>
+  <si>
+    <t>Raw value one side</t>
+  </si>
+  <si>
+    <t>Raw value both sides</t>
+  </si>
+  <si>
+    <t>Ponderated value both sides</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Min-Max</t>
+  </si>
+  <si>
+    <t>Alpha-Beta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,14 +140,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,6 +166,427 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" fmlaLink="$B$26" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$A$26" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Option Button 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>209550</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>514350</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Option Button 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Group Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Option Button 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Option Button 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C56AFD-CC19-4907-91F6-E40EE6A69B8D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="Option Button 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ACFD5B8-BFCA-4D3C-BDFF-7B50286A075C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,157 +851,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Feuil1"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -561,7 +1014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -569,10 +1022,201 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="H19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId4" name="Option Button 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor>
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId5" name="Option Button 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>209550</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId6" name="Group Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" r:id="rId7" name="Option Button 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1043" r:id="rId8" name="Option Button 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1045" r:id="rId9" name="Option Button 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix et comparaison perfs
</commit_message>
<xml_diff>
--- a/tsume-configuration.xlsx
+++ b/tsume-configuration.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mes docs\Documents\Mes documents\home\quicklisp\local-projects\TsumeLi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\home\quicklisp\local-projects\TsumeLi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8866D-7CDA-44AC-A20E-0FB9414A2806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA89B6B-0634-4BFF-B3BC-E8C5B4259679}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5708" yWindow="3173" windowWidth="16875" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Ce tableur permet la saisie de la configuration du tsume qui sera résolu par le programme TsumeLi</t>
   </si>
@@ -48,21 +48,6 @@
     <t>-L</t>
   </si>
   <si>
-    <t>-B</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>+L</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>-P</t>
   </si>
   <si>
@@ -85,24 +70,31 @@
   </si>
   <si>
     <t>Alpha-Beta</t>
+  </si>
+  <si>
+    <t>-N</t>
+  </si>
+  <si>
+    <t>-S</t>
+  </si>
+  <si>
+    <t>-G</t>
+  </si>
+  <si>
+    <t>+B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,11 +161,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" fmlaLink="$B$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$B$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,7 +467,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C56AFD-CC19-4907-91F6-E40EE6A69B8D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -542,7 +534,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ACFD5B8-BFCA-4D3C-BDFF-7B50286A075C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -856,17 +848,17 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="B19" sqref="B19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -880,77 +872,87 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -960,7 +962,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -969,11 +971,9 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -984,7 +984,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -995,7 +995,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1006,64 +1006,61 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="H19" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>